<commit_message>
Planilha de medição atualizada
</commit_message>
<xml_diff>
--- a/artefatos/Planilha de Medição - Grupo 1.xlsx
+++ b/artefatos/Planilha de Medição - Grupo 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>Medição de software</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Responsável</t>
   </si>
   <si>
-    <t>Dados obtidos através da ferramenta Sonar Qube</t>
-  </si>
-  <si>
-    <t>Dados obtidos do relatório de testes.</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -182,6 +176,15 @@
   </si>
   <si>
     <t>Valores determinados comparando-se as tarefas do processo no RedMine e as atividades definidas no Scrub</t>
+  </si>
+  <si>
+    <t>Observações - V1</t>
+  </si>
+  <si>
+    <t>Atualização dos Requsitos, Depuração, Diagrama de Sequência, Coletar Informações sobre Regras de Negócio</t>
+  </si>
+  <si>
+    <t>Renan</t>
   </si>
   <si>
     <r>
@@ -202,8 +205,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 1</t>
+      <t xml:space="preserve"> 1. Não foram realizados testes, de modo que a tabela do índice de defeitos encontrados na fase de testes (In_Df) encontra-se sem informações até o momento.</t>
     </r>
+  </si>
+  <si>
+    <t>Observações - Versão 1</t>
+  </si>
+  <si>
+    <t>Observações - Versão 2</t>
+  </si>
+  <si>
+    <t>Requisitos não atendidos: RFs 5, 9, 10, 13, 15, 16, 17, 18, 19, 22</t>
+  </si>
+  <si>
+    <t>No número de tarefas, foram desconsideradas as 2 tarefas de entrega de artefatos e do sistema.</t>
+  </si>
+  <si>
+    <t>Quantidades obtidas pelo RedMine</t>
   </si>
 </sst>
 </file>
@@ -211,7 +229,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$R$-416]\ #,##0.00;[Red]\-[$R$-416]\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$R$-416]\ #,##0.00;[Red]\-[$R$-416]\ #,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -409,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -430,17 +448,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -473,27 +485,6 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="12" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -503,7 +494,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -512,6 +503,30 @@
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -524,11 +539,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,10 +715,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,6 +759,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -742,11 +778,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="391123576"/>
-        <c:axId val="391121616"/>
+        <c:axId val="325227976"/>
+        <c:axId val="325222096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="391123576"/>
+        <c:axId val="325227976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391121616"/>
+        <c:crossAx val="325222096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -764,7 +800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391121616"/>
+        <c:axId val="325222096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391123576"/>
+        <c:crossAx val="325227976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -905,11 +941,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391115344"/>
-        <c:axId val="391112208"/>
+        <c:axId val="325224056"/>
+        <c:axId val="326814752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391115344"/>
+        <c:axId val="325224056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +963,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="391112208"/>
+        <c:crossAx val="326814752"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -936,7 +972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391112208"/>
+        <c:axId val="326814752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +1017,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391115344"/>
+        <c:crossAx val="325224056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1103,12 +1139,18 @@
             <c:strRef>
               <c:f>G_RF!$E$4:$H$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Versão 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Versão 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Observações - Versão 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Observações - Versão 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1120,7 +1162,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.29411764705882354</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1171,12 +1213,18 @@
             <c:strRef>
               <c:f>G_RF!$E$4:$H$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Versão 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Versão 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Observações - Versão 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Observações - Versão 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1188,7 +1236,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.29411764705882354</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1208,11 +1256,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391114560"/>
-        <c:axId val="391110640"/>
+        <c:axId val="326817888"/>
+        <c:axId val="326815536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391114560"/>
+        <c:axId val="326817888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1278,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="391110640"/>
+        <c:crossAx val="326815536"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1287,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391110640"/>
+        <c:axId val="326815536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1332,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="391114560"/>
+        <c:crossAx val="326817888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1386,10 +1434,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65217391304347827</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,11 +1452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="391118088"/>
-        <c:axId val="391112600"/>
+        <c:axId val="326821808"/>
+        <c:axId val="326819064"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="391118088"/>
+        <c:axId val="326821808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,7 +1466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391112600"/>
+        <c:crossAx val="326819064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1427,7 +1475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391112600"/>
+        <c:axId val="326819064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1486,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391118088"/>
+        <c:crossAx val="326821808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,15 +1508,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1626250</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>489103</xdr:rowOff>
+      <xdr:colOff>1385256</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>213681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>837740</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>103283</xdr:rowOff>
+      <xdr:colOff>596746</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57379</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1953,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:G12"/>
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1964,22 +2012,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="4" spans="3:7" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
     </row>
     <row r="5" spans="3:7" ht="18" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
@@ -1995,12 +2043,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="18" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2028,36 +2076,34 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="3:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="C11" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="3:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="3:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C11:G13"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2072,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2084,7 +2130,7 @@
     <col min="4" max="4" width="91.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
@@ -2093,34 +2139,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
+      <c r="B1" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="B2" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" ht="33.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -2128,18 +2174,18 @@
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -2155,7 +2201,9 @@
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -2164,72 +2212,92 @@
     </row>
     <row r="5" spans="1:12" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="33">
+        <v>7</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+    </row>
+    <row r="6" spans="1:12" ht="90.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="34">
+        <v>4</v>
+      </c>
+      <c r="F6" s="34">
+        <v>0</v>
+      </c>
+      <c r="G6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="42">
-        <v>10</v>
-      </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="43">
-        <v>7</v>
-      </c>
-      <c r="F6" s="43">
-        <v>0</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="37"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" ht="56.85" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C7" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="24">
+        <v>43024</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" ht="56.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="44"/>
+      <c r="D8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
     <row r="9" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2246,7 +2314,7 @@
   <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2260,41 +2328,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="33" t="s">
+      <c r="D3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2317,88 +2385,84 @@
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="17">
+        <v>42</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="15">
         <v>0</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="15">
         <v>0</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="17">
+        <v>41</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="15">
         <v>0</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>0</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="20" t="e">
+      <c r="B7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="18" t="e">
         <f>E5/E6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F7" s="20" t="e">
+      <c r="F7" s="18" t="e">
         <f>F5/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C8" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="26">
-        <v>42917</v>
-      </c>
-      <c r="F8" s="26">
-        <v>42959</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="C8" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="24">
+        <v>43024</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C9" s="45"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="E9" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2424,7 +2488,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2433,46 +2497,46 @@
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" style="4" customWidth="1"/>
-    <col min="5" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="33" t="s">
+      <c r="D3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -2490,93 +2554,91 @@
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="17">
+        <v>37</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="15">
         <v>10</v>
       </c>
-      <c r="F5" s="17">
-        <v>0</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="17">
-        <v>34</v>
-      </c>
-      <c r="F6" s="17">
-        <v>0</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+        <v>38</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="15">
+        <v>22</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="50"/>
     </row>
     <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24">
+      <c r="B7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22">
         <f>E5/E6</f>
-        <v>0.29411764705882354</v>
-      </c>
-      <c r="F7" s="24" t="e">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F7" s="22" t="e">
         <f>F5/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="26">
+      <c r="C8" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="24">
         <v>42917</v>
       </c>
-      <c r="F8" s="26">
-        <v>42959</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="45"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="E9" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C10"/>
@@ -2584,12 +2646,14 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2605,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2615,31 +2679,31 @@
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" style="4" customWidth="1"/>
-    <col min="5" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -2647,14 +2711,14 @@
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -2670,103 +2734,107 @@
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="17">
-        <v>10</v>
-      </c>
-      <c r="F5" s="17">
-        <v>15</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="15">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="15">
+        <v>33</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="18">
+        <f>E5/E6</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F7" s="18" t="e">
+        <f>F5/F6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="C8" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="17">
-        <v>20</v>
-      </c>
-      <c r="F6" s="17">
-        <v>23</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="20">
-        <f>E5/E6</f>
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="20">
-        <f>F5/F6</f>
-        <v>0.65217391304347827</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C8" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="26">
+      <c r="E8" s="24">
         <v>42917</v>
       </c>
-      <c r="F8" s="26">
-        <v>42959</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C9" s="45"/>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="E9" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="7">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>